<commit_message>
modified:   Enter/enter_config.json 	modified:   Enter/enter_test_info.xlsx 	modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx 	modified:   test.cpp
</commit_message>
<xml_diff>
--- a/Enter/enter_test_info.xlsx
+++ b/Enter/enter_test_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="10905"/>
+    <workbookView windowWidth="17400" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="矿" sheetId="12" r:id="rId1"/>
@@ -152,13 +152,10 @@
     <t>锁僵尸位置</t>
   </si>
   <si>
-    <t>最快</t>
+    <t>随机</t>
   </si>
   <si>
     <t>锁植物反应</t>
-  </si>
-  <si>
-    <t>最慢</t>
   </si>
   <si>
     <t>灰烬范围(上小下大)</t>
@@ -167,10 +164,13 @@
     <t>橄</t>
   </si>
   <si>
-    <t>跳</t>
+    <t>最快</t>
   </si>
   <si>
-    <t>随机</t>
+    <t>最慢</t>
+  </si>
+  <si>
+    <t>跳</t>
   </si>
   <si>
     <t>梯</t>
@@ -1372,7 +1372,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -1463,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>1466</v>
+        <v>1634</v>
       </c>
       <c r="K3" s="6"/>
       <c r="M3" s="3"/>
@@ -1477,7 +1477,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>16</v>
@@ -1750,7 +1750,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -2110,7 +2110,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="5">
         <v>5</v>
@@ -2250,7 +2250,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -2266,7 +2266,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -2626,7 +2626,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="5">
         <v>5</v>
@@ -2766,7 +2766,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -2782,7 +2782,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -3285,7 +3285,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -3301,7 +3301,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -3799,7 +3799,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -3815,7 +3815,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -3828,7 +3828,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -4313,7 +4313,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -4329,7 +4329,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -4342,7 +4342,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -4829,7 +4829,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -4845,7 +4845,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -4858,7 +4858,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -5345,7 +5345,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -5361,7 +5361,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>

</xml_diff>

<commit_message>
modified:   Enter/enter_config.json 	modified:   Enter/enter_test_info.xlsx 	modified:   "\347\275\256\344\277\241\345\214\272\351\227\264\344\270\216\345\201\207\350\256\276\346\243\200\351\252\214.ipynb"
</commit_message>
<xml_diff>
--- a/Enter/enter_test_info.xlsx
+++ b/Enter/enter_test_info.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="17400" windowHeight="8760"/>
+    <workbookView windowWidth="14925" windowHeight="10005"/>
   </bookViews>
   <sheets>
-    <sheet name="矿" sheetId="12" r:id="rId1"/>
-    <sheet name="橄" sheetId="6" r:id="rId2"/>
-    <sheet name="跳" sheetId="9" r:id="rId3"/>
-    <sheet name="梯" sheetId="11" r:id="rId4"/>
-    <sheet name="豚" sheetId="8" r:id="rId5"/>
-    <sheet name="潜" sheetId="7" r:id="rId6"/>
+    <sheet name="豚" sheetId="8" r:id="rId1"/>
+    <sheet name="潜" sheetId="7" r:id="rId2"/>
+    <sheet name="矿" sheetId="12" r:id="rId3"/>
+    <sheet name="跳" sheetId="9" r:id="rId4"/>
+    <sheet name="梯" sheetId="11" r:id="rId5"/>
+    <sheet name="橄" sheetId="6" r:id="rId6"/>
     <sheet name="篮球投率" sheetId="10" r:id="rId7"/>
     <sheet name="红白" sheetId="5" r:id="rId8"/>
   </sheets>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="51">
   <si>
     <t>小丑类型</t>
   </si>
@@ -89,13 +89,10 @@
     <t>曾</t>
   </si>
   <si>
-    <t>永动</t>
+    <t>非永动</t>
   </si>
   <si>
     <t>被炸植物列数</t>
-  </si>
-  <si>
-    <t>非永动</t>
   </si>
   <si>
     <t>被炸植物类型</t>
@@ -113,16 +110,13 @@
     <t>已有伤害</t>
   </si>
   <si>
-    <t>喷</t>
-  </si>
-  <si>
     <t>冰瓜额外溅射次数</t>
   </si>
   <si>
     <t>僵尸类型</t>
   </si>
   <si>
-    <t>矿</t>
+    <t>豚</t>
   </si>
   <si>
     <t>测试次数</t>
@@ -143,7 +137,7 @@
     <t>灰烬类型</t>
   </si>
   <si>
-    <t>卡</t>
+    <t>炮</t>
   </si>
   <si>
     <t>植物可伤时机</t>
@@ -161,13 +155,22 @@
     <t>灰烬范围(上小下大)</t>
   </si>
   <si>
-    <t>橄</t>
+    <t>潜</t>
   </si>
   <si>
-    <t>最快</t>
+    <t>永动</t>
+  </si>
+  <si>
+    <t>卡</t>
   </si>
   <si>
     <t>最慢</t>
+  </si>
+  <si>
+    <t>喷</t>
+  </si>
+  <si>
+    <t>矿</t>
   </si>
   <si>
     <t>跳</t>
@@ -176,16 +179,10 @@
     <t>梯</t>
   </si>
   <si>
-    <t>豚</t>
-  </si>
-  <si>
-    <t>潜</t>
+    <t>橄</t>
   </si>
   <si>
     <t>篮球投率</t>
-  </si>
-  <si>
-    <t>炮</t>
   </si>
   <si>
     <t>红</t>
@@ -198,13 +195,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="&quot;￥&quot;#,##0.00_);[Red]\(&quot;￥&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +352,13 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -670,7 +675,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -818,8 +823,11 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -844,8 +852,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
     <cellStyle name="货币" xfId="2" builtinId="4"/>
@@ -895,6 +906,7 @@
     <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Neutral 2" xfId="49"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1368,10 +1380,1041 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="7" width="9.23333333333333" style="2"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.23333333333333" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="13" width="11.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.9833333333333" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.23333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:14">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:14">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:14">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:14">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:14">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:14">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:14">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:14">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:14">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:14">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6">
+        <v>10000000</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:14">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="4:14">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:14">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1476</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:14">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6">
+        <v>6000</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:14">
+      <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:14">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="4:14">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:14">
+      <c r="A18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:14">
+      <c r="A19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:14">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="6">
+        <v>473</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="I20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:14">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6">
+        <v>743</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="4:14">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="4:14">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="4:14">
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="4:14">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6 F7 F8 F3:F5 F9:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7 E8 E9 E3:E6 E10:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet23"/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="7" width="9.23333333333333" style="2"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.23333333333333" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="13" width="11.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.9833333333333" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.23333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:14">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:14">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:14">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:14">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:14">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:14">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:14">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:14">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:14">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="5">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:14">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:14">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="4:14">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:14">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="6">
+        <v>100</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:14">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6">
+        <v>5000</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:14">
+      <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:14">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="4:14">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:14">
+      <c r="A18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:14">
+      <c r="A19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:14">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="6">
+        <v>100</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="I20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:14">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6">
+        <v>101</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="4:14">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="4:14">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="4:14">
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="4:14">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D9 D10:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6 F7 F8 F9 F3:F5 F10:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7 E8 E9 E3:E6 E10:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -1457,13 +2500,13 @@
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G3" s="5">
         <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>1634</v>
+        <v>1617</v>
       </c>
       <c r="K3" s="6"/>
       <c r="M3" s="3"/>
@@ -1483,10 +2526,10 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I4" s="6"/>
       <c r="K4" s="6"/>
@@ -1495,10 +2538,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:14">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="5">
         <v>6</v>
@@ -1507,7 +2550,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -1519,10 +2562,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:14">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="5">
         <v>6</v>
@@ -1531,7 +2574,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -1543,7 +2586,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -1552,10 +2595,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -1567,7 +2610,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:14">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -1576,10 +2619,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -1591,19 +2634,19 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D9" s="5">
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -1615,10 +2658,10 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1631,10 +2674,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1657,7 +2700,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6">
         <v>0</v>
@@ -1673,10 +2716,10 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1689,10 +2732,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1705,7 +2748,7 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -1731,10 +2774,10 @@
     </row>
     <row r="18" s="1" customFormat="1" spans="1:14">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1747,10 +2790,10 @@
     </row>
     <row r="19" s="1" customFormat="1" spans="1:14">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1763,7 +2806,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -1883,19 +2926,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet14"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23333333333333" style="1"/>
+    <col min="2" max="2" width="9.375" style="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
     <col min="4" max="7" width="9.23333333333333" style="2"/>
     <col min="8" max="8" width="9.23333333333333" style="1"/>
     <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
@@ -1967,7 +3011,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>16</v>
@@ -1976,10 +3020,10 @@
         <v>17</v>
       </c>
       <c r="G3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="6">
-        <v>1433</v>
+        <v>774</v>
       </c>
       <c r="K3" s="6"/>
       <c r="M3" s="3"/>
@@ -1993,16 +3037,16 @@
         <v>9</v>
       </c>
       <c r="D4" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="6"/>
       <c r="K4" s="6"/>
@@ -2011,19 +3055,19 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:14">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D5" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -2035,19 +3079,19 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:14">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -2059,7 +3103,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -2068,10 +3112,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -2083,7 +3127,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:14">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -2092,10 +3136,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -2107,19 +3151,19 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D9" s="5">
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -2131,10 +3175,10 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -2147,10 +3191,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -2173,10 +3217,10 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -2189,10 +3233,10 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -2205,10 +3249,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -2221,7 +3265,7 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2247,10 +3291,10 @@
     </row>
     <row r="18" s="1" customFormat="1" spans="1:14">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -2263,10 +3307,10 @@
     </row>
     <row r="19" s="1" customFormat="1" spans="1:14">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -2279,7 +3323,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -2399,19 +3443,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23333333333333" style="1"/>
+    <col min="2" max="2" width="9.375" style="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
     <col min="4" max="7" width="9.23333333333333" style="2"/>
     <col min="8" max="8" width="9.23333333333333" style="1"/>
     <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
@@ -2489,13 +3534,13 @@
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="5">
         <v>1</v>
       </c>
       <c r="I3" s="6">
-        <v>774</v>
+        <v>783</v>
       </c>
       <c r="K3" s="6"/>
       <c r="M3" s="3"/>
@@ -2515,22 +3560,25 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="6">
+        <f>I3+2501</f>
+        <v>3284</v>
+      </c>
       <c r="K4" s="6"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:14">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="5">
         <v>4</v>
@@ -2539,7 +3587,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -2551,10 +3599,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:14">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
@@ -2563,7 +3611,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -2575,7 +3623,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -2584,10 +3632,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -2599,7 +3647,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:14">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -2608,10 +3656,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -2623,19 +3671,19 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" s="5">
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -2647,10 +3695,10 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -2663,10 +3711,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -2689,7 +3737,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6">
         <v>100</v>
@@ -2705,10 +3753,10 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -2721,10 +3769,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -2737,7 +3785,7 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2763,10 +3811,10 @@
     </row>
     <row r="18" s="1" customFormat="1" spans="1:14">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -2779,10 +3827,10 @@
     </row>
     <row r="19" s="1" customFormat="1" spans="1:14">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -2795,7 +3843,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -2915,19 +3963,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet12"/>
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23333333333333" style="1"/>
+    <col min="2" max="2" width="9.375" style="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
     <col min="4" max="7" width="9.23333333333333" style="2"/>
     <col min="8" max="8" width="9.23333333333333" style="1"/>
     <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
@@ -2999,19 +4048,19 @@
         <v>15</v>
       </c>
       <c r="D3" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="G3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>100</v>
+        <v>830</v>
       </c>
       <c r="K3" s="6"/>
       <c r="M3" s="3"/>
@@ -3025,20 +4074,20 @@
         <v>9</v>
       </c>
       <c r="D4" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="G4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="6">
         <f>I3+2501</f>
-        <v>2601</v>
+        <v>3331</v>
       </c>
       <c r="K4" s="6"/>
       <c r="M4" s="3"/>
@@ -3046,22 +4095,22 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:14">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D5" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="6"/>
       <c r="K5" s="6"/>
@@ -3070,19 +4119,19 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:14">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -3094,7 +4143,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -3103,10 +4152,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -3118,7 +4167,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:14">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -3127,10 +4176,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -3142,19 +4191,19 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9" s="5">
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -3166,10 +4215,10 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6">
-        <v>2000000</v>
+        <v>10000000</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -3182,10 +4231,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -3208,10 +4257,10 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -3224,7 +4273,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6">
         <v>6000</v>
@@ -3240,10 +4289,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -3256,7 +4305,7 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -3282,10 +4331,10 @@
     </row>
     <row r="18" s="1" customFormat="1" spans="1:14">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -3298,10 +4347,10 @@
     </row>
     <row r="19" s="1" customFormat="1" spans="1:14">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -3314,7 +4363,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -3434,1040 +4483,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="7" width="9.23333333333333" style="2"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.23333333333333" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="13" width="11.375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.9833333333333" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.23333333333333" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:14">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:14">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:14">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:14">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:14">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:14">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:14">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>7</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:14">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>6</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:14">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="5">
-        <v>5</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:14">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:14">
-      <c r="A11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="I11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="4:14">
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:14">
-      <c r="A13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="6">
-        <v>100</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:14">
-      <c r="A14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="6">
-        <v>5000</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:14">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:14">
-      <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="4:14">
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" s="1" customFormat="1" spans="1:14">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="1:14">
-      <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="1:14">
-      <c r="A20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="6">
-        <v>100</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="1:14">
-      <c r="A21" s="3"/>
-      <c r="B21" s="6">
-        <v>101</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="4:14">
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="4:14">
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="I23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="4:14">
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="4:14">
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="I25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
-      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet23"/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="7" width="9.23333333333333" style="2"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.23333333333333" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="13" width="11.375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.9833333333333" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.23333333333333" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:14">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:14">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:14">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:14">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:14">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:14">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5">
-        <v>6</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:14">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>7</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:14">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>6</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:14">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="5">
-        <v>5</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:14">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:14">
-      <c r="A11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="I11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="4:14">
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:14">
-      <c r="A13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="6">
-        <v>100</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:14">
-      <c r="A14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="6">
-        <v>5000</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:14">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:14">
-      <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="4:14">
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" s="1" customFormat="1" spans="1:14">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="1:14">
-      <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="1:14">
-      <c r="A20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="6">
-        <v>100</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="1:14">
-      <c r="A21" s="3"/>
-      <c r="B21" s="6">
-        <v>101</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="4:14">
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="4:14">
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="I23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="4:14">
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="4:14">
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="I25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
-      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -4552,7 +4573,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="5">
         <v>0</v>
@@ -4578,7 +4599,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
@@ -4590,10 +4611,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:14">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="5">
         <v>4</v>
@@ -4602,7 +4623,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -4614,10 +4635,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:14">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
@@ -4626,7 +4647,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -4638,7 +4659,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -4647,10 +4668,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -4662,7 +4683,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:14">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -4671,10 +4692,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -4686,7 +4707,7 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>48</v>
@@ -4695,10 +4716,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -4710,7 +4731,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6">
         <v>1000000</v>
@@ -4726,10 +4747,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -4752,7 +4773,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6">
         <v>1729</v>
@@ -4768,7 +4789,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6">
         <v>3000</v>
@@ -4784,10 +4805,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -4800,7 +4821,7 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -4826,10 +4847,10 @@
     </row>
     <row r="18" s="1" customFormat="1" spans="1:14">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -4842,10 +4863,10 @@
     </row>
     <row r="19" s="1" customFormat="1" spans="1:14">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -4858,7 +4879,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="6">
         <v>100</v>
@@ -4984,7 +5005,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -5068,7 +5089,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="5">
         <v>0</v>
@@ -5094,7 +5115,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
@@ -5106,10 +5127,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:14">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="5">
         <v>6</v>
@@ -5118,7 +5139,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -5130,10 +5151,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:14">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="5">
         <v>6</v>
@@ -5142,7 +5163,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -5154,7 +5175,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -5163,10 +5184,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -5178,7 +5199,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:14">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -5187,10 +5208,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -5202,19 +5223,19 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="5">
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -5226,7 +5247,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6">
         <v>1000000</v>
@@ -5242,10 +5263,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -5268,7 +5289,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6">
         <v>916</v>
@@ -5284,7 +5305,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6">
         <v>15000</v>
@@ -5300,10 +5321,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -5316,7 +5337,7 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -5342,10 +5363,10 @@
     </row>
     <row r="18" s="1" customFormat="1" spans="1:14">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -5358,10 +5379,10 @@
     </row>
     <row r="19" s="1" customFormat="1" spans="1:14">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -5374,7 +5395,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
deleted:    Catapult/README.md 	deleted:    Catapult/catapult_config.json 	deleted:    Catapult/help.ipynb 	renamed:    Catapult/Catapult_cpp_1_0.cpp -> Enter/Catapult/Catapult_cpp_1_0.cpp 	new file:   Enter/Catapult/help.ipynb 	modified:   Enter/enter_config.json 	modified:   Enter/enter_test_info.xlsx 	renamed:    "\345\217\214\346\233\276\346\274\217\350\267\263\350\267\263\346\246\202\347\216\207\350\256\241\347\256\227.ipynb" -> "\346\235\202/\345\217\214\346\233\276\346\274\217\350\267\263\350\267\263\346\246\202\347\216\207\350\256\241\347\256\227.ipynb" 	renamed:    "\347\214\264\347\211\210\347\240\270\347\216\207\350\256\241\347\256\227.ipynb" -> "\346\235\202/\347\214\264\347\211\210\347\240\270\347\216\207\350\256\241\347\256\227.ipynb" 	deleted:    "\346\235\202/\350\256\241\345\210\222\344\271\246.md"
</commit_message>
<xml_diff>
--- a/Enter/enter_test_info.xlsx
+++ b/Enter/enter_test_info.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="48">
   <si>
     <t>小丑类型</t>
   </si>
@@ -98,9 +98,6 @@
     <t>非永动</t>
   </si>
   <si>
-    <t>炮</t>
-  </si>
-  <si>
     <t>被炸植物列数</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>随机</t>
+  </si>
+  <si>
+    <t>炮</t>
   </si>
   <si>
     <t>跳</t>
@@ -353,7 +353,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,12 +381,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,12 +464,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -513,12 +501,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,7 +691,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -733,16 +715,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -751,92 +733,92 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -865,9 +847,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1402,7 +1381,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -1505,22 +1484,14 @@
         <v>1</v>
       </c>
       <c r="K3" s="8"/>
-      <c r="M3" s="8">
-        <v>1728</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="10">
-        <v>100</v>
-      </c>
-      <c r="P3" s="10">
-        <v>900</v>
-      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -1541,15 +1512,15 @@
       <c r="K4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="7">
         <v>4</v>
@@ -1567,15 +1538,15 @@
       <c r="K5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -1584,7 +1555,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -1593,12 +1564,12 @@
       <c r="K6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -1607,7 +1578,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -1619,12 +1590,12 @@
       <c r="K7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -1633,10 +1604,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -1645,24 +1616,24 @@
       <c r="K8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="D9" s="7">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -1671,12 +1642,12 @@
       <c r="K9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>1000000</v>
@@ -1689,15 +1660,15 @@
       <c r="K10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1707,8 +1678,8 @@
       <c r="K11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:16">
       <c r="D12" s="7"/>
@@ -1719,12 +1690,12 @@
       <c r="K12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -1737,15 +1708,15 @@
       <c r="K13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1755,15 +1726,15 @@
       <c r="K14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1773,15 +1744,15 @@
       <c r="K15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1791,8 +1762,8 @@
       <c r="K16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="4:16">
       <c r="D17" s="7"/>
@@ -1803,8 +1774,8 @@
       <c r="K17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:16">
       <c r="D18" s="7"/>
@@ -1815,8 +1786,8 @@
       <c r="K18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="4:16">
       <c r="D19" s="7"/>
@@ -1827,8 +1798,8 @@
       <c r="K19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="4:16">
       <c r="D20" s="7"/>
@@ -1839,8 +1810,8 @@
       <c r="K20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="4:16">
       <c r="D21" s="7"/>
@@ -1851,8 +1822,8 @@
       <c r="K21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="4:16">
       <c r="D22" s="7"/>
@@ -1863,8 +1834,8 @@
       <c r="K22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="4:16">
       <c r="D23" s="7"/>
@@ -1875,8 +1846,8 @@
       <c r="K23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="4:16">
       <c r="D24" s="7"/>
@@ -1887,8 +1858,8 @@
       <c r="K24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="4:16">
       <c r="D25" s="7"/>
@@ -1899,8 +1870,8 @@
       <c r="K25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2064,18 +2035,18 @@
         <v>1039</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="10">
+        <v>40</v>
+      </c>
+      <c r="O3" s="8">
         <v>100</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="8">
         <v>900</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -2096,15 +2067,15 @@
       <c r="K4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="7">
         <v>5</v>
@@ -2122,15 +2093,15 @@
       <c r="K5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -2139,7 +2110,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -2148,12 +2119,12 @@
       <c r="K6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -2162,7 +2133,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -2174,12 +2145,12 @@
       <c r="K7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -2188,10 +2159,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -2200,12 +2171,12 @@
       <c r="K8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>41</v>
@@ -2214,10 +2185,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -2226,12 +2197,12 @@
       <c r="K9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>10000000</v>
@@ -2244,15 +2215,15 @@
       <c r="K10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -2262,8 +2233,8 @@
       <c r="K11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:16">
       <c r="D12" s="7"/>
@@ -2274,12 +2245,12 @@
       <c r="K12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -2292,12 +2263,12 @@
       <c r="K13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -2310,15 +2281,15 @@
       <c r="K14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -2328,15 +2299,15 @@
       <c r="K15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -2346,8 +2317,8 @@
       <c r="K16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="4:16">
       <c r="D17" s="7"/>
@@ -2358,8 +2329,8 @@
       <c r="K17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:16">
       <c r="D18" s="7"/>
@@ -2370,8 +2341,8 @@
       <c r="K18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="4:16">
       <c r="D19" s="7"/>
@@ -2382,8 +2353,8 @@
       <c r="K19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="4:16">
       <c r="D20" s="7"/>
@@ -2394,8 +2365,8 @@
       <c r="K20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="4:16">
       <c r="D21" s="7"/>
@@ -2406,8 +2377,8 @@
       <c r="K21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="4:16">
       <c r="D22" s="7"/>
@@ -2418,8 +2389,8 @@
       <c r="K22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="4:16">
       <c r="D23" s="7"/>
@@ -2430,8 +2401,8 @@
       <c r="K23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="4:16">
       <c r="D24" s="7"/>
@@ -2442,8 +2413,8 @@
       <c r="K24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="4:16">
       <c r="D25" s="7"/>
@@ -2454,8 +2425,8 @@
       <c r="K25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2475,9 +2446,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3 N4:N25">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
@@ -2501,6 +2469,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
       <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
+      <formula1>"卡,炮"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2619,12 +2590,12 @@
       <c r="K3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -2645,15 +2616,15 @@
       <c r="K4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="7">
         <v>4</v>
@@ -2671,15 +2642,15 @@
       <c r="K5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -2697,12 +2668,12 @@
       <c r="K6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -2723,12 +2694,12 @@
       <c r="K7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -2749,12 +2720,12 @@
       <c r="K8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>42</v>
@@ -2775,12 +2746,12 @@
       <c r="K9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>10000000</v>
@@ -2793,15 +2764,15 @@
       <c r="K10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -2811,8 +2782,8 @@
       <c r="K11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:16">
       <c r="D12" s="7"/>
@@ -2823,12 +2794,12 @@
       <c r="K12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -2841,12 +2812,12 @@
       <c r="K13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -2859,15 +2830,15 @@
       <c r="K14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -2877,15 +2848,15 @@
       <c r="K15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -2895,8 +2866,8 @@
       <c r="K16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="4:16">
       <c r="D17" s="7"/>
@@ -2907,8 +2878,8 @@
       <c r="K17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:16">
       <c r="D18" s="7"/>
@@ -2919,8 +2890,8 @@
       <c r="K18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="4:16">
       <c r="D19" s="7"/>
@@ -2931,8 +2902,8 @@
       <c r="K19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="4:16">
       <c r="D20" s="7"/>
@@ -2943,8 +2914,8 @@
       <c r="K20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="4:16">
       <c r="D21" s="7"/>
@@ -2955,8 +2926,8 @@
       <c r="K21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="4:16">
       <c r="D22" s="7"/>
@@ -2967,8 +2938,8 @@
       <c r="K22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="4:16">
       <c r="D23" s="7"/>
@@ -2979,8 +2950,8 @@
       <c r="K23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="4:16">
       <c r="D24" s="7"/>
@@ -2991,8 +2962,8 @@
       <c r="K24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="4:16">
       <c r="D25" s="7"/>
@@ -3003,8 +2974,8 @@
       <c r="K25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3166,12 +3137,12 @@
       <c r="K3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -3192,15 +3163,15 @@
       <c r="K4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="7">
         <v>4</v>
@@ -3218,15 +3189,15 @@
       <c r="K5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -3244,12 +3215,12 @@
       <c r="K6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -3270,12 +3241,12 @@
       <c r="K7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -3286,7 +3257,7 @@
       <c r="E8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="7">
@@ -3296,12 +3267,12 @@
       <c r="K8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>43</v>
@@ -3313,7 +3284,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7">
         <v>1</v>
@@ -3322,12 +3293,12 @@
       <c r="K9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>1000000</v>
@@ -3340,15 +3311,15 @@
       <c r="K10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -3358,8 +3329,8 @@
       <c r="K11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:16">
       <c r="D12" s="7"/>
@@ -3370,12 +3341,12 @@
       <c r="K12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -3388,12 +3359,12 @@
       <c r="K13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -3406,15 +3377,15 @@
       <c r="K14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -3424,15 +3395,15 @@
       <c r="K15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -3442,8 +3413,8 @@
       <c r="K16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="4:16">
       <c r="D17" s="7"/>
@@ -3454,8 +3425,8 @@
       <c r="K17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:16">
       <c r="D18" s="7"/>
@@ -3466,8 +3437,8 @@
       <c r="K18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="4:16">
       <c r="D19" s="7"/>
@@ -3478,8 +3449,8 @@
       <c r="K19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="4:16">
       <c r="D20" s="7"/>
@@ -3490,8 +3461,8 @@
       <c r="K20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="4:16">
       <c r="D21" s="7"/>
@@ -3502,8 +3473,8 @@
       <c r="K21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="4:16">
       <c r="D22" s="7"/>
@@ -3514,8 +3485,8 @@
       <c r="K22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="4:16">
       <c r="D23" s="7"/>
@@ -3526,8 +3497,8 @@
       <c r="K23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="4:16">
       <c r="D24" s="7"/>
@@ -3538,8 +3509,8 @@
       <c r="K24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="4:16">
       <c r="D25" s="7"/>
@@ -3550,8 +3521,8 @@
       <c r="K25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3704,7 +3675,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="7">
         <v>0</v>
@@ -3715,12 +3686,12 @@
       <c r="K3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -3741,15 +3712,15 @@
       <c r="K4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="7">
         <v>6</v>
@@ -3758,7 +3729,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -3767,15 +3738,15 @@
       <c r="K5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -3784,7 +3755,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -3793,12 +3764,12 @@
       <c r="K6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -3807,7 +3778,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -3819,12 +3790,12 @@
       <c r="K7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -3833,10 +3804,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -3845,12 +3816,12 @@
       <c r="K8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>44</v>
@@ -3859,10 +3830,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -3871,12 +3842,12 @@
       <c r="K9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>1000000</v>
@@ -3889,15 +3860,15 @@
       <c r="K10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -3907,8 +3878,8 @@
       <c r="K11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:16">
       <c r="D12" s="7"/>
@@ -3919,12 +3890,12 @@
       <c r="K12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -3937,12 +3908,12 @@
       <c r="K13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -3955,15 +3926,15 @@
       <c r="K14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -3973,15 +3944,15 @@
       <c r="K15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -3991,8 +3962,8 @@
       <c r="K16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="4:16">
       <c r="D17" s="7"/>
@@ -4003,8 +3974,8 @@
       <c r="K17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:16">
       <c r="D18" s="7"/>
@@ -4015,8 +3986,8 @@
       <c r="K18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="4:16">
       <c r="D19" s="7"/>
@@ -4027,8 +3998,8 @@
       <c r="K19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="4:16">
       <c r="D20" s="7"/>
@@ -4039,8 +4010,8 @@
       <c r="K20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="4:16">
       <c r="D21" s="7"/>
@@ -4051,8 +4022,8 @@
       <c r="K21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="4:16">
       <c r="D22" s="7"/>
@@ -4063,8 +4034,8 @@
       <c r="K22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="4:16">
       <c r="D23" s="7"/>
@@ -4075,8 +4046,8 @@
       <c r="K23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="4:16">
       <c r="D24" s="7"/>
@@ -4087,8 +4058,8 @@
       <c r="K24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="4:16">
       <c r="D25" s="7"/>
@@ -4099,8 +4070,8 @@
       <c r="K25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4264,12 +4235,12 @@
       <c r="K3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -4293,15 +4264,15 @@
       <c r="K4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="7">
         <v>4</v>
@@ -4310,7 +4281,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -4319,15 +4290,15 @@
       <c r="K5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -4336,7 +4307,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -4345,12 +4316,12 @@
       <c r="K6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -4359,7 +4330,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -4371,12 +4342,12 @@
       <c r="K7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -4385,10 +4356,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -4397,12 +4368,12 @@
       <c r="K8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>45</v>
@@ -4411,10 +4382,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -4423,12 +4394,12 @@
       <c r="K9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>10000000</v>
@@ -4441,15 +4412,15 @@
       <c r="K10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -4459,8 +4430,8 @@
       <c r="K11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:16">
       <c r="D12" s="7"/>
@@ -4471,12 +4442,12 @@
       <c r="K12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -4489,12 +4460,12 @@
       <c r="K13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -4507,15 +4478,15 @@
       <c r="K14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -4525,15 +4496,15 @@
       <c r="K15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -4543,8 +4514,8 @@
       <c r="K16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="4:16">
       <c r="D17" s="7"/>
@@ -4555,8 +4526,8 @@
       <c r="K17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:16">
       <c r="D18" s="7"/>
@@ -4567,8 +4538,8 @@
       <c r="K18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="4:16">
       <c r="D19" s="7"/>
@@ -4579,8 +4550,8 @@
       <c r="K19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="4:16">
       <c r="D20" s="7"/>
@@ -4591,8 +4562,8 @@
       <c r="K20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="4:16">
       <c r="D21" s="7"/>
@@ -4603,8 +4574,8 @@
       <c r="K21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="4:16">
       <c r="D22" s="7"/>
@@ -4615,8 +4586,8 @@
       <c r="K22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="4:16">
       <c r="D23" s="7"/>
@@ -4627,8 +4598,8 @@
       <c r="K23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="4:16">
       <c r="D24" s="7"/>
@@ -4639,8 +4610,8 @@
       <c r="K24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="4:16">
       <c r="D25" s="7"/>
@@ -4651,8 +4622,8 @@
       <c r="K25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4805,7 +4776,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="7">
         <v>0</v>
@@ -4816,12 +4787,12 @@
       <c r="K3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -4833,7 +4804,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="7">
         <v>1</v>
@@ -4845,15 +4816,15 @@
       <c r="K4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="7">
         <v>6</v>
@@ -4862,7 +4833,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="7">
         <v>1</v>
@@ -4871,15 +4842,15 @@
       <c r="K5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -4888,7 +4859,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -4897,12 +4868,12 @@
       <c r="K6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -4911,7 +4882,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -4923,12 +4894,12 @@
       <c r="K7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -4937,10 +4908,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -4949,12 +4920,12 @@
       <c r="K8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>46</v>
@@ -4963,10 +4934,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -4975,12 +4946,12 @@
       <c r="K9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>10000000</v>
@@ -4993,15 +4964,15 @@
       <c r="K10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -5011,8 +4982,8 @@
       <c r="K11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:16">
       <c r="D12" s="7"/>
@@ -5023,12 +4994,12 @@
       <c r="K12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -5041,12 +5012,12 @@
       <c r="K13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -5059,15 +5030,15 @@
       <c r="K14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -5077,15 +5048,15 @@
       <c r="K15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -5095,8 +5066,8 @@
       <c r="K16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="4:16">
       <c r="D17" s="7"/>
@@ -5107,8 +5078,8 @@
       <c r="K17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:16">
       <c r="D18" s="7"/>
@@ -5119,8 +5090,8 @@
       <c r="K18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="4:16">
       <c r="D19" s="7"/>
@@ -5131,8 +5102,8 @@
       <c r="K19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="4:16">
       <c r="D20" s="7"/>
@@ -5143,8 +5114,8 @@
       <c r="K20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="4:16">
       <c r="D21" s="7"/>
@@ -5155,8 +5126,8 @@
       <c r="K21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="4:16">
       <c r="D22" s="7"/>
@@ -5167,8 +5138,8 @@
       <c r="K22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="4:16">
       <c r="D23" s="7"/>
@@ -5179,8 +5150,8 @@
       <c r="K23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="4:16">
       <c r="D24" s="7"/>
@@ -5191,8 +5162,8 @@
       <c r="K24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="4:16">
       <c r="D25" s="7"/>
@@ -5203,8 +5174,8 @@
       <c r="K25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5368,12 +5339,12 @@
       <c r="K3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -5394,15 +5365,15 @@
       <c r="K4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="7">
         <v>6</v>
@@ -5411,7 +5382,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -5420,15 +5391,15 @@
       <c r="K5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -5437,7 +5408,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -5446,12 +5417,12 @@
       <c r="K6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -5460,7 +5431,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -5472,12 +5443,12 @@
       <c r="K7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -5486,10 +5457,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -5498,12 +5469,12 @@
       <c r="K8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>47</v>
@@ -5512,10 +5483,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -5524,12 +5495,12 @@
       <c r="K9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>1000000</v>
@@ -5542,15 +5513,15 @@
       <c r="K10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -5560,8 +5531,8 @@
       <c r="K11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:16">
       <c r="D12" s="7"/>
@@ -5572,12 +5543,12 @@
       <c r="K12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -5590,12 +5561,12 @@
       <c r="K13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -5608,15 +5579,15 @@
       <c r="K14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -5626,15 +5597,15 @@
       <c r="K15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -5644,8 +5615,8 @@
       <c r="K16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="4:16">
       <c r="D17" s="7"/>
@@ -5656,8 +5627,8 @@
       <c r="K17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:16">
       <c r="D18" s="7"/>
@@ -5668,8 +5639,8 @@
       <c r="K18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="4:16">
       <c r="D19" s="7"/>
@@ -5680,8 +5651,8 @@
       <c r="K19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="4:16">
       <c r="D20" s="7"/>
@@ -5692,8 +5663,8 @@
       <c r="K20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="4:16">
       <c r="D21" s="7"/>
@@ -5704,8 +5675,8 @@
       <c r="K21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="4:16">
       <c r="D22" s="7"/>
@@ -5716,8 +5687,8 @@
       <c r="K22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="4:16">
       <c r="D23" s="7"/>
@@ -5728,8 +5699,8 @@
       <c r="K23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="4:16">
       <c r="D24" s="7"/>
@@ -5740,8 +5711,8 @@
       <c r="K24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="4:16">
       <c r="D25" s="7"/>
@@ -5752,8 +5723,8 @@
       <c r="K25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
new file:   Enter/Position/Position_cpp_1_0.cpp 	modified:   Enter/enter_config.json 	modified:   Enter/enter_test_info.xlsx 	modified:   inc/calculate_position.hpp 	modified:   inc/tools/Enter.hpp 	modified:   inc/tools/Jack.hpp 	modified:   inc/tools/Zomboni.hpp 	modified:   output.csv 	modified:   test.cpp
</commit_message>
<xml_diff>
--- a/Enter/enter_test_info.xlsx
+++ b/Enter/enter_test_info.xlsx
@@ -7,14 +7,14 @@
     <workbookView windowWidth="27750" windowHeight="10665"/>
   </bookViews>
   <sheets>
-    <sheet name="篮球投率" sheetId="10" r:id="rId1"/>
-    <sheet name="跳" sheetId="9" r:id="rId2"/>
-    <sheet name="豚" sheetId="8" r:id="rId3"/>
-    <sheet name="潜" sheetId="7" r:id="rId4"/>
-    <sheet name="矿" sheetId="12" r:id="rId5"/>
-    <sheet name="梯" sheetId="11" r:id="rId6"/>
-    <sheet name="橄" sheetId="6" r:id="rId7"/>
-    <sheet name="红白" sheetId="5" r:id="rId8"/>
+    <sheet name="红白" sheetId="5" r:id="rId1"/>
+    <sheet name="篮球投率" sheetId="10" r:id="rId2"/>
+    <sheet name="跳" sheetId="9" r:id="rId3"/>
+    <sheet name="豚" sheetId="8" r:id="rId4"/>
+    <sheet name="潜" sheetId="7" r:id="rId5"/>
+    <sheet name="矿" sheetId="12" r:id="rId6"/>
+    <sheet name="梯" sheetId="11" r:id="rId7"/>
+    <sheet name="橄" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -107,13 +107,13 @@
     <t>普通</t>
   </si>
   <si>
+    <t>永动</t>
+  </si>
+  <si>
     <t>波次类型</t>
   </si>
   <si>
     <t>通常波</t>
-  </si>
-  <si>
-    <t>永动</t>
   </si>
   <si>
     <t>已有伤害</t>
@@ -128,7 +128,7 @@
     <t>僵尸类型</t>
   </si>
   <si>
-    <t>篮球投率</t>
+    <t>红</t>
   </si>
   <si>
     <t>测试次数</t>
@@ -158,6 +158,9 @@
     <t>随机</t>
   </si>
   <si>
+    <t>篮球投率</t>
+  </si>
+  <si>
     <t>炮</t>
   </si>
   <si>
@@ -177,9 +180,6 @@
   </si>
   <si>
     <t>橄</t>
-  </si>
-  <si>
-    <t>红</t>
   </si>
 </sst>
 </file>
@@ -1377,11 +1377,560 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:P25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="25.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="6" width="8.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.23333333333333" style="1"/>
+    <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="14" width="5.125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.23333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:16">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:16">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="M2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:16">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8">
+        <v>40</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:16">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:16">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="7">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:16">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:16">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:16">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>6</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:16">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:16">
+      <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="I10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:16">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:16">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="I12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:16">
+      <c r="A13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="I13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:16">
+      <c r="A14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="8">
+        <v>5000</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:16">
+      <c r="A15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="I15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:16">
+      <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="I16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="4:16">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="4:16">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="I18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="4:16">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="I19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="4:16">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="4:16">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="I21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="4:16">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="I22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="4:16">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="I23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="4:16">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="I24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="4:16">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="I25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -1543,10 +2092,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -1555,7 +2104,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -1607,7 +2156,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -1624,7 +2173,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D9" s="7">
         <v>5</v>
@@ -1633,7 +2182,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -1924,7 +2473,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P25"/>
@@ -2035,7 +2584,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O3" s="8">
         <v>100</v>
@@ -2098,10 +2647,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -2110,7 +2659,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -2162,7 +2711,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -2179,7 +2728,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="7">
         <v>5</v>
@@ -2188,7 +2737,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -2479,7 +3028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P25"/>
@@ -2647,10 +3196,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -2728,7 +3277,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="7">
         <v>9</v>
@@ -3028,7 +3577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:P25"/>
@@ -3194,10 +3743,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -3275,7 +3824,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="7">
         <v>9</v>
@@ -3284,7 +3833,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G9" s="7">
         <v>1</v>
@@ -3575,7 +4124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P25"/>
@@ -3675,7 +4224,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" s="7">
         <v>0</v>
@@ -3729,7 +4278,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -3743,10 +4292,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -3755,7 +4304,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -3807,7 +4356,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -3824,7 +4373,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="7">
         <v>5</v>
@@ -3833,7 +4382,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -4124,7 +4673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:P25"/>
@@ -4281,7 +4830,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -4295,10 +4844,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -4307,7 +4856,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -4359,7 +4908,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -4376,7 +4925,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D9" s="7">
         <v>5</v>
@@ -4385,7 +4934,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -4676,7 +5225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:P25"/>
@@ -4776,7 +5325,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" s="7">
         <v>0</v>
@@ -4804,7 +5353,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G4" s="7">
         <v>1</v>
@@ -4833,7 +5382,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G5" s="7">
         <v>1</v>
@@ -4847,10 +5396,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -4859,7 +5408,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -4911,7 +5460,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -4928,7 +5477,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" s="7">
         <v>5</v>
@@ -4937,7 +5486,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -5226,553 +5775,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:P25"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="25.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="6" width="8.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.23333333333333" style="1"/>
-    <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="14" width="5.125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.23333333333333" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:16">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:16">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:16">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="K3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:16">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:16">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7">
-        <v>6</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:16">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="7">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:16">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:16">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7">
-        <v>6</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:16">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="7">
-        <v>5</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:16">
-      <c r="A10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="I10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:16">
-      <c r="A11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:16">
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="I12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:16">
-      <c r="A13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="I13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:16">
-      <c r="A14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="8">
-        <v>5000</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:16">
-      <c r="A15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="I15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:16">
-      <c r="A16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="I16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="4:16">
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-    </row>
-    <row r="18" s="1" customFormat="1" spans="4:16">
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="I18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="4:16">
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="I19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="4:16">
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="4:16">
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="I21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="4:16">
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="I22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="4:16">
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="I23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="4:16">
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="I24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="4:16">
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="I25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
-      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   Enter/enter_config.json 	modified:   Enter/enter_test_info.xlsx
</commit_message>
<xml_diff>
--- a/Enter/enter_test_info.xlsx
+++ b/Enter/enter_test_info.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27750" windowHeight="10665"/>
+    <workbookView windowWidth="20610" windowHeight="7275"/>
   </bookViews>
   <sheets>
-    <sheet name="红白" sheetId="5" r:id="rId1"/>
-    <sheet name="篮球投率" sheetId="10" r:id="rId2"/>
-    <sheet name="跳" sheetId="9" r:id="rId3"/>
-    <sheet name="豚" sheetId="8" r:id="rId4"/>
-    <sheet name="潜" sheetId="7" r:id="rId5"/>
+    <sheet name="潜" sheetId="7" r:id="rId1"/>
+    <sheet name="豚" sheetId="8" r:id="rId2"/>
+    <sheet name="红白" sheetId="5" r:id="rId3"/>
+    <sheet name="篮球投率" sheetId="10" r:id="rId4"/>
+    <sheet name="跳" sheetId="9" r:id="rId5"/>
     <sheet name="矿" sheetId="12" r:id="rId6"/>
     <sheet name="梯" sheetId="11" r:id="rId7"/>
     <sheet name="橄" sheetId="6" r:id="rId8"/>
@@ -107,9 +107,6 @@
     <t>普通</t>
   </si>
   <si>
-    <t>永动</t>
-  </si>
-  <si>
     <t>波次类型</t>
   </si>
   <si>
@@ -119,16 +116,16 @@
     <t>已有伤害</t>
   </si>
   <si>
-    <t>喷</t>
-  </si>
-  <si>
     <t>冰瓜额外溅射次数</t>
   </si>
   <si>
     <t>僵尸类型</t>
   </si>
   <si>
-    <t>红</t>
+    <t>潜</t>
+  </si>
+  <si>
+    <t>永动</t>
   </si>
   <si>
     <t>测试次数</t>
@@ -149,13 +146,22 @@
     <t>锁僵尸出生点与冻结倒计时</t>
   </si>
   <si>
-    <t>最快</t>
+    <t>随机</t>
   </si>
   <si>
     <t>锁植物攻击间隔</t>
   </si>
   <si>
-    <t>随机</t>
+    <t>豚</t>
+  </si>
+  <si>
+    <t>喷</t>
+  </si>
+  <si>
+    <t>红</t>
+  </si>
+  <si>
+    <t>最快</t>
   </si>
   <si>
     <t>篮球投率</t>
@@ -165,12 +171,6 @@
   </si>
   <si>
     <t>跳</t>
-  </si>
-  <si>
-    <t>豚</t>
-  </si>
-  <si>
-    <t>潜</t>
   </si>
   <si>
     <t>矿</t>
@@ -1377,10 +1377,1106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet23"/>
+  <dimension ref="A1:P25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="25.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="6" width="8.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.23333333333333" style="1"/>
+    <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="14" width="5.125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.23333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:16">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:16">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="M2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:16">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>3000</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:16">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:16">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="7">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:16">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:16">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:16">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:16">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:16">
+      <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="I10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:16">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:16">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="I12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:16">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="I13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:16">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="8">
+        <v>6000</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:16">
+      <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="I15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:16">
+      <c r="A16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="I16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="4:16">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="4:16">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="I18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="4:16">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="I19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="4:16">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="4:16">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="I21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="4:16">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="I22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="4:16">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="I23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="4:16">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="I24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="4:16">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="I25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:P25"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D$1:G$1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="25.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="6" width="8.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.23333333333333" style="1"/>
+    <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="14" width="5.125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.23333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:16">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:16">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="M2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:16">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:16">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:16">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="7">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:16">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:16">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:16">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:16">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:16">
+      <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="I10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:16">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:16">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="I12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:16">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="I13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:16">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="8">
+        <v>5000</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:16">
+      <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="I15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:16">
+      <c r="A16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="I16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="4:16">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="4:16">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="I18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="4:16">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="I19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="4:16">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="4:16">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="I21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="4:16">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="I22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="4:16">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="I23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="4:16">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="I24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="4:16">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="I25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1529,7 +2625,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -1543,10 +2639,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -1555,7 +2651,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -1569,7 +2665,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -1578,7 +2674,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -1595,7 +2691,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -1604,10 +2700,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -1621,19 +2717,19 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D9" s="7">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -1647,7 +2743,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8">
         <v>1000000</v>
@@ -1665,10 +2761,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1695,7 +2791,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -1713,7 +2809,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -1731,10 +2827,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1749,10 +2845,10 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1924,7 +3020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P25"/>
@@ -2092,10 +3188,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -2104,7 +3200,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -2118,7 +3214,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -2127,7 +3223,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -2144,7 +3240,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -2153,10 +3249,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -2170,19 +3266,19 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D9" s="7">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -2196,7 +3292,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8">
         <v>1000000</v>
@@ -2214,10 +3310,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -2244,7 +3340,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -2262,7 +3358,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8">
         <v>3000</v>
@@ -2280,10 +3376,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -2298,10 +3394,10 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -2473,7 +3569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P25"/>
@@ -2584,7 +3680,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O3" s="8">
         <v>100</v>
@@ -2647,10 +3743,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -2659,7 +3755,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -2673,7 +3769,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -2682,7 +3778,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -2699,7 +3795,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -2708,10 +3804,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -2725,19 +3821,19 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D9" s="7">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -2751,7 +3847,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8">
         <v>10000000</v>
@@ -2769,10 +3865,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -2799,7 +3895,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -2817,7 +3913,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -2835,10 +3931,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -2853,1106 +3949,10 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="I16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="4:16">
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-    </row>
-    <row r="18" s="1" customFormat="1" spans="4:16">
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="I18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="4:16">
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="I19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="4:16">
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="4:16">
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="I21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="4:16">
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="I22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="4:16">
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="I23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="4:16">
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="I24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="4:16">
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="I25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
-      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P25"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="25.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="6" width="8.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.23333333333333" style="1"/>
-    <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="14" width="5.125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.23333333333333" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:16">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:16">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:16">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="K3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:16">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7">
-        <v>3</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:16">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7">
-        <v>4</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:16">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:16">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:16">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7">
-        <v>8</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:16">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="7">
-        <v>9</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:16">
-      <c r="A10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="8">
-        <v>10000000</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="I10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:16">
-      <c r="A11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:16">
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="I12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:16">
-      <c r="A13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="I13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:16">
-      <c r="A14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="8">
-        <v>5000</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:16">
-      <c r="A15" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="I15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:16">
-      <c r="A16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="I16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="4:16">
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-    </row>
-    <row r="18" s="1" customFormat="1" spans="4:16">
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="I18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="4:16">
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="I19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="4:16">
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="4:16">
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="I21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="4:16">
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="I22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="4:16">
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="I23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="4:16">
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="I24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="4:16">
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="I25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
-      <formula1>"杆,报,门,橄,潜,车,豚,丑,气,矿,跳,梯,篮,白,红,篮球投率"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet23"/>
-  <dimension ref="A1:P25"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="25.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="6" width="8.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.23333333333333" style="1"/>
-    <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="14" width="5.125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.23333333333333" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:16">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:16">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:16">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="7">
-        <v>2</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:16">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:16">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7">
-        <v>4</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:16">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="7">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:16">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="7">
-        <v>2</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:16">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7">
-        <v>8</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:16">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="7">
-        <v>9</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:16">
-      <c r="A10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="I10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:16">
-      <c r="A11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:16">
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="I12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:16">
-      <c r="A13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="I13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:16">
-      <c r="A14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="8">
-        <v>5000</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:16">
-      <c r="A15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="I15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:16">
-      <c r="A16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -4224,7 +4224,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G3" s="7">
         <v>0</v>
@@ -4278,7 +4278,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -4292,10 +4292,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -4304,7 +4304,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -4318,7 +4318,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -4327,7 +4327,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -4344,7 +4344,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -4353,10 +4353,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>45</v>
@@ -4379,10 +4379,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8">
         <v>1000000</v>
@@ -4414,10 +4414,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -4462,7 +4462,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -4480,10 +4480,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -4498,10 +4498,10 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -4830,7 +4830,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -4844,10 +4844,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -4856,7 +4856,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -4879,7 +4879,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -4905,10 +4905,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -4922,7 +4922,7 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>46</v>
@@ -4931,10 +4931,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -4948,7 +4948,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8">
         <v>10000000</v>
@@ -4966,10 +4966,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -4996,7 +4996,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -5014,7 +5014,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -5032,10 +5032,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -5050,10 +5050,10 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -5325,7 +5325,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G3" s="7">
         <v>0</v>
@@ -5353,7 +5353,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G4" s="7">
         <v>1</v>
@@ -5382,7 +5382,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G5" s="7">
         <v>1</v>
@@ -5396,10 +5396,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>6</v>
@@ -5408,7 +5408,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -5422,7 +5422,7 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -5431,7 +5431,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -5448,7 +5448,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -5457,10 +5457,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -5474,7 +5474,7 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>47</v>
@@ -5483,10 +5483,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -5500,7 +5500,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8">
         <v>10000000</v>
@@ -5518,10 +5518,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -5548,7 +5548,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -5566,7 +5566,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8">
         <v>5000</v>
@@ -5584,10 +5584,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -5602,10 +5602,10 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>

</xml_diff>